<commit_message>
updated example status spreadsheet
</commit_message>
<xml_diff>
--- a/doc/status.xlsx
+++ b/doc/status.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="95">
   <si>
     <t>Example</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>Text output</t>
-  </si>
-  <si>
-    <t>segfault every time</t>
   </si>
   <si>
     <t>test state machine</t>
@@ -635,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,10 +671,10 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,7 +732,7 @@
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,7 +751,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
         <v>67</v>
@@ -768,7 +765,7 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,7 +820,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -831,13 +828,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
         <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,7 +1017,7 @@
         <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" t="s">
         <v>67</v>
@@ -1031,7 +1028,7 @@
         <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
         <v>68</v>
@@ -1042,7 +1039,7 @@
         <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
         <v>67</v>
@@ -1053,7 +1050,7 @@
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
         <v>67</v>
@@ -1067,13 +1064,13 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" t="s">
         <v>85</v>
-      </c>
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,13 +1078,13 @@
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
         <v>77</v>
-      </c>
-      <c r="D40" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1095,13 +1092,13 @@
         <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" t="s">
         <v>67</v>
       </c>
       <c r="D41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1109,13 +1106,13 @@
         <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
         <v>67</v>
       </c>
       <c r="D42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,7 +1120,7 @@
         <v>56</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" t="s">
         <v>67</v>
@@ -1145,13 +1142,13 @@
         <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
         <v>67</v>
       </c>
       <c r="D46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1159,7 +1156,7 @@
         <v>59</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
         <v>67</v>
@@ -1170,7 +1167,7 @@
         <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
         <v>67</v>
@@ -1181,7 +1178,7 @@
         <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
         <v>67</v>
@@ -1192,13 +1189,13 @@
         <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
         <v>67</v>
       </c>
       <c r="D50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,13 +1203,13 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
         <v>67</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1226,7 +1223,7 @@
         <v>67</v>
       </c>
       <c r="D52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1240,7 +1237,7 @@
         <v>67</v>
       </c>
       <c r="D53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>